<commit_message>
19/10/2022 generic libraries implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sncsr\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project videos\VtigerCRM\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{681EE748-1F06-4B9C-B2E1-5B239559109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ADB8AC-C4D5-422C-81E1-0B70D3CD75F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6492B4B-4497-484C-9067-5A512381FFD5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -65,9 +65,6 @@
     <t/>
   </si>
   <si>
-    <t>Create Oganization</t>
-  </si>
-  <si>
     <t>Organization Name</t>
   </si>
   <si>
@@ -123,12 +120,19 @@
   </si>
   <si>
     <t>XYZ</t>
+  </si>
+  <si>
+    <t>Create Organization</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -606,17 +610,17 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="14.109375"/>
+    <col min="2" max="2" customWidth="true" style="1" width="37.88671875"/>
+    <col min="3" max="3" customWidth="true" style="1" width="29.21875"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.33203125"/>
+    <col min="5" max="5" customWidth="true" style="1" width="16.88671875"/>
+    <col min="6" max="16384" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -641,25 +645,27 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2"/>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -667,10 +673,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -706,13 +712,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E7"/>
     </row>
@@ -721,10 +727,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E8"/>
     </row>
@@ -733,19 +739,19 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -781,13 +787,13 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E13"/>
     </row>
@@ -796,19 +802,19 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Generic Utility implementation and POM page for login page for reference
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project videos\VtigerCRM\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ADB8AC-C4D5-422C-81E1-0B70D3CD75F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06079400-3019-4737-A7D2-4C605B5A426E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6492B4B-4497-484C-9067-5A512381FFD5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>New Last Name</t>
+  </si>
+  <si>
+    <t>Cde</t>
   </si>
 </sst>
 </file>
@@ -297,8 +303,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E96E555A-892F-4E24-B3E4-B10DD02D5B8E}" name="Table36" displayName="Table36" ref="A12:E16" totalsRowShown="0">
-  <autoFilter ref="A12:E16" xr:uid="{E96E555A-892F-4E24-B3E4-B10DD02D5B8E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E96E555A-892F-4E24-B3E4-B10DD02D5B8E}" name="Table36" displayName="Table36" ref="A12:E17" totalsRowShown="0">
+  <autoFilter ref="A12:E17" xr:uid="{E96E555A-892F-4E24-B3E4-B10DD02D5B8E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B2E3D6C-36AF-4210-9240-F23500B2F12D}" name="Test Case_ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{8FE930CF-94CC-4870-A74A-88780D32421F}" name="TestCase Name" dataDxfId="3" dataCellStyle="Hyperlink"/>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62DB3FF2-2714-4A0C-BD43-CF27AE3038AE}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,7 +726,9 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7"/>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -795,7 +803,9 @@
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13"/>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
@@ -818,13 +828,22 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Maven command line parameters practice
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>TestCase Name</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Cde</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -804,7 +807,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>